<commit_message>
102/GFG. Level Order Traversal
102/GFG. Level Order Traversal
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List.xlsx
+++ b/Binary Search Tree/Java/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDD66BB-B627-460B-BBCF-CC4A95FFD251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EA75-648D-4318-965D-BDFBABD862A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
   <si>
     <t>Question No</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Java/Python</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
   </si>
 </sst>
 </file>
@@ -523,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,224 +597,227 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>701</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>216</v>
+        <v>700</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>938</v>
+        <v>216</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>104</v>
+        <v>938</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>104</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>199</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>110</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>543</v>
-      </c>
-      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
-        <v>17</v>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>543</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>100</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>124</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>101</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>103</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>236</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
+        <v>236</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>662</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -821,76 +827,73 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>226</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>297</v>
+        <v>226</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>105</v>
+        <v>297</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
+        <v>222</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>106</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -901,35 +904,35 @@
         <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>235</v>
+      <c r="A33" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>114</v>
+        <v>235</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -943,18 +946,21 @@
         <v>41</v>
       </c>
       <c r="D35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>114</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,28 +968,39 @@
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>450</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
+        <v>450</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
         <v>98</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PostOrder Traversal using 2 stack approach
PostOrder Traversal using 2 stack approach
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Java/Question_List.xlsx
+++ b/Binary Search Tree/Java/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Binary Search Tree\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EA75-648D-4318-965D-BDFBABD862A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C500B882-59E8-4C0F-9841-A43670C98AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Minimum element in BST (Find min and max value in a BST)</t>
   </si>
   <si>
-    <t>Binary Tree Postorder Traversal-Recursive</t>
-  </si>
-  <si>
     <t>Binary Tree Preorder Traversal-Recursive</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal-Recursive,Iterative(2 Stack and 1 Stack approach)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -564,10 +564,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>145</v>
       </c>
@@ -575,10 +575,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,10 +589,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,13 +600,13 @@
         <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,10 +647,10 @@
         <v>938</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,10 +658,10 @@
         <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>199</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,10 +702,10 @@
         <v>110</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,10 +713,10 @@
         <v>543</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -735,10 +735,10 @@
         <v>124</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,10 +746,10 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,10 +768,10 @@
         <v>103</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,10 +790,10 @@
         <v>236</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,18 +804,18 @@
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="6"/>
     </row>
@@ -827,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -857,10 +857,10 @@
         <v>297</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,10 +879,10 @@
         <v>222</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,35 +893,35 @@
         <v>7</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -943,10 +943,10 @@
         <v>7</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -957,32 +957,32 @@
         <v>7</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
         <v>41</v>
-      </c>
-      <c r="D36" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,10 +990,10 @@
         <v>450</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>